<commit_message>
Criação dos métodos de adicionar e remover ferramenta
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,102 +421,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr"/>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-    </row>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:A7"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>